<commit_message>
Added code to calculate the total singapore population by subzone
</commit_message>
<xml_diff>
--- a/merged_subzone_population.xlsx
+++ b/merged_subzone_population.xlsx
@@ -468,7 +468,7 @@
         <v>103.8085594783731</v>
       </c>
       <c r="D2" t="n">
-        <v>2730</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         <v>103.8185897231269</v>
       </c>
       <c r="D3" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         <v>103.8436874187531</v>
       </c>
       <c r="D4" t="n">
-        <v>4700</v>
+        <v>10080</v>
       </c>
     </row>
     <row r="5">
@@ -515,10 +515,8 @@
       <c r="C5" t="n">
         <v>103.8486541763248</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -533,10 +531,8 @@
       <c r="C6" t="n">
         <v>103.8510073819891</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D6" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -552,7 +548,7 @@
         <v>103.8468833241059</v>
       </c>
       <c r="D7" t="n">
-        <v>640</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="8">
@@ -568,7 +564,7 @@
         <v>103.8313927594441</v>
       </c>
       <c r="D8" t="n">
-        <v>5790</v>
+        <v>12130</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +598,7 @@
         <v>103.8268263612172</v>
       </c>
       <c r="D10" t="n">
-        <v>6020</v>
+        <v>14570</v>
       </c>
     </row>
     <row r="11">
@@ -654,7 +650,7 @@
         <v>103.8641870281905</v>
       </c>
       <c r="D13" t="n">
-        <v>500</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14">
@@ -688,7 +684,7 @@
         <v>103.8375003969992</v>
       </c>
       <c r="D15" t="n">
-        <v>3310</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="16">
@@ -704,7 +700,7 @@
         <v>103.8370641286037</v>
       </c>
       <c r="D16" t="n">
-        <v>4030</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="17">
@@ -719,10 +715,8 @@
       <c r="C17" t="n">
         <v>103.6986386515527</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D17" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -738,7 +732,7 @@
         <v>103.8460529566889</v>
       </c>
       <c r="D18" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19">
@@ -754,7 +748,7 @@
         <v>103.8394225451616</v>
       </c>
       <c r="D19" t="n">
-        <v>3330</v>
+        <v>5110</v>
       </c>
     </row>
     <row r="20">
@@ -770,7 +764,7 @@
         <v>103.8481890611351</v>
       </c>
       <c r="D20" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21">
@@ -786,7 +780,7 @@
         <v>103.8223827838929</v>
       </c>
       <c r="D21" t="n">
-        <v>6000</v>
+        <v>12770</v>
       </c>
     </row>
     <row r="22">
@@ -802,7 +796,7 @@
         <v>103.817163352372</v>
       </c>
       <c r="D22" t="n">
-        <v>5260</v>
+        <v>10980</v>
       </c>
     </row>
     <row r="23">
@@ -818,7 +812,7 @@
         <v>103.8095865142582</v>
       </c>
       <c r="D23" t="n">
-        <v>5410</v>
+        <v>12880</v>
       </c>
     </row>
     <row r="24">
@@ -834,7 +828,7 @@
         <v>103.830443810365</v>
       </c>
       <c r="D24" t="n">
-        <v>6430</v>
+        <v>13430</v>
       </c>
     </row>
     <row r="25">
@@ -849,10 +843,8 @@
       <c r="C25" t="n">
         <v>103.8445791656904</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D25" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="26">
@@ -868,7 +860,7 @@
         <v>103.7801010738711</v>
       </c>
       <c r="D26" t="n">
-        <v>2860</v>
+        <v>4750</v>
       </c>
     </row>
     <row r="27">
@@ -884,7 +876,7 @@
         <v>103.7989117871098</v>
       </c>
       <c r="D27" t="n">
-        <v>150</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28">
@@ -972,7 +964,7 @@
         <v>103.8296691638396</v>
       </c>
       <c r="D32" t="n">
-        <v>2160</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="33">
@@ -987,10 +979,8 @@
       <c r="C33" t="n">
         <v>103.8368005527159</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D33" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="34">
@@ -1006,7 +996,7 @@
         <v>103.8436099596135</v>
       </c>
       <c r="D34" t="n">
-        <v>240</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35">
@@ -1040,7 +1030,7 @@
         <v>103.8136228311552</v>
       </c>
       <c r="D36" t="n">
-        <v>3100</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="37">
@@ -1056,7 +1046,7 @@
         <v>103.8246027826011</v>
       </c>
       <c r="D37" t="n">
-        <v>4790</v>
+        <v>11530</v>
       </c>
     </row>
     <row r="38">
@@ -1072,7 +1062,7 @@
         <v>103.8458786023595</v>
       </c>
       <c r="D38" t="n">
-        <v>1980</v>
+        <v>940</v>
       </c>
     </row>
     <row r="39">
@@ -1088,7 +1078,7 @@
         <v>103.836315892199</v>
       </c>
       <c r="D39" t="n">
-        <v>4420</v>
+        <v>7510</v>
       </c>
     </row>
     <row r="40">
@@ -1104,7 +1094,7 @@
         <v>103.8204741470173</v>
       </c>
       <c r="D40" t="n">
-        <v>3950</v>
+        <v>8330</v>
       </c>
     </row>
     <row r="41">
@@ -1138,7 +1128,7 @@
         <v>103.8488650609934</v>
       </c>
       <c r="D42" t="n">
-        <v>1330</v>
+        <v>540</v>
       </c>
     </row>
     <row r="43">
@@ -1154,7 +1144,7 @@
         <v>103.827350765752</v>
       </c>
       <c r="D43" t="n">
-        <v>4850</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="44">
@@ -1170,7 +1160,7 @@
         <v>103.8088798405162</v>
       </c>
       <c r="D44" t="n">
-        <v>7860</v>
+        <v>19100</v>
       </c>
     </row>
     <row r="45">
@@ -1186,7 +1176,7 @@
         <v>103.7946153341631</v>
       </c>
       <c r="D45" t="n">
-        <v>1850</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="46">
@@ -1202,7 +1192,7 @@
         <v>103.8524200008228</v>
       </c>
       <c r="D46" t="n">
-        <v>2800</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="47">
@@ -1236,7 +1226,7 @@
         <v>103.8560367975615</v>
       </c>
       <c r="D48" t="n">
-        <v>1600</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="49">
@@ -1252,7 +1242,7 @@
         <v>103.8529896159258</v>
       </c>
       <c r="D49" t="n">
-        <v>920</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="50">
@@ -1268,7 +1258,7 @@
         <v>103.8316052065549</v>
       </c>
       <c r="D50" t="n">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51">
@@ -1301,10 +1291,8 @@
       <c r="C52" t="n">
         <v>103.7766186493374</v>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D52" t="n">
+        <v>290</v>
       </c>
     </row>
     <row r="53">
@@ -1320,7 +1308,7 @@
         <v>103.8271685672495</v>
       </c>
       <c r="D53" t="n">
-        <v>1750</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="54">
@@ -1336,7 +1324,7 @@
         <v>103.7998816749111</v>
       </c>
       <c r="D54" t="n">
-        <v>3410</v>
+        <v>6550</v>
       </c>
     </row>
     <row r="55">
@@ -1352,7 +1340,7 @@
         <v>103.7795494476269</v>
       </c>
       <c r="D55" t="n">
-        <v>4450</v>
+        <v>11290</v>
       </c>
     </row>
     <row r="56">
@@ -1368,7 +1356,7 @@
         <v>103.8114690598696</v>
       </c>
       <c r="D56" t="n">
-        <v>820</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="57">
@@ -1384,7 +1372,7 @@
         <v>103.8376503825013</v>
       </c>
       <c r="D57" t="n">
-        <v>3830</v>
+        <v>4630</v>
       </c>
     </row>
     <row r="58">
@@ -1400,7 +1388,7 @@
         <v>103.7630913920634</v>
       </c>
       <c r="D58" t="n">
-        <v>7530</v>
+        <v>14540</v>
       </c>
     </row>
     <row r="59">
@@ -1416,7 +1404,7 @@
         <v>103.8416029635527</v>
       </c>
       <c r="D59" t="n">
-        <v>740</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="60">
@@ -1432,7 +1420,7 @@
         <v>103.9270861597486</v>
       </c>
       <c r="D60" t="n">
-        <v>3590</v>
+        <v>7390</v>
       </c>
     </row>
     <row r="61">
@@ -1448,7 +1436,7 @@
         <v>103.7683186628504</v>
       </c>
       <c r="D61" t="n">
-        <v>8050</v>
+        <v>18860</v>
       </c>
     </row>
     <row r="62">
@@ -1463,10 +1451,8 @@
       <c r="C62" t="n">
         <v>103.6614548137725</v>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D62" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="63">
@@ -1481,10 +1467,8 @@
       <c r="C63" t="n">
         <v>103.7403368942165</v>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D63" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="64">
@@ -1500,7 +1484,7 @@
         <v>103.8303370525791</v>
       </c>
       <c r="D64" t="n">
-        <v>1810</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="65">
@@ -1516,7 +1500,7 @@
         <v>103.870495873079</v>
       </c>
       <c r="D65" t="n">
-        <v>830</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="66">
@@ -1532,7 +1516,7 @@
         <v>103.7925683646149</v>
       </c>
       <c r="D66" t="n">
-        <v>1920</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="67">
@@ -1548,7 +1532,7 @@
         <v>103.820274155872</v>
       </c>
       <c r="D67" t="n">
-        <v>1870</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="68">
@@ -1564,7 +1548,7 @@
         <v>103.796755556588</v>
       </c>
       <c r="D68" t="n">
-        <v>5570</v>
+        <v>5880</v>
       </c>
     </row>
     <row r="69">
@@ -1580,7 +1564,7 @@
         <v>103.8484143355784</v>
       </c>
       <c r="D69" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70">
@@ -1596,7 +1580,7 @@
         <v>103.8566928831913</v>
       </c>
       <c r="D70" t="n">
-        <v>890</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="71">
@@ -1612,7 +1596,7 @@
         <v>103.7909112050153</v>
       </c>
       <c r="D71" t="n">
-        <v>1150</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="72">
@@ -1628,7 +1612,7 @@
         <v>103.8759107061609</v>
       </c>
       <c r="D72" t="n">
-        <v>5540</v>
+        <v>11460</v>
       </c>
     </row>
     <row r="73">
@@ -1644,7 +1628,7 @@
         <v>103.9023351117397</v>
       </c>
       <c r="D73" t="n">
-        <v>4350</v>
+        <v>9450</v>
       </c>
     </row>
     <row r="74">
@@ -1660,7 +1644,7 @@
         <v>103.8325721300139</v>
       </c>
       <c r="D74" t="n">
-        <v>710</v>
+        <v>540</v>
       </c>
     </row>
     <row r="75">
@@ -1675,10 +1659,8 @@
       <c r="C75" t="n">
         <v>103.8443422082146</v>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D75" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="76">
@@ -1694,7 +1676,7 @@
         <v>103.8540526534276</v>
       </c>
       <c r="D76" t="n">
-        <v>1200</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="77">
@@ -1727,10 +1709,8 @@
       <c r="C78" t="n">
         <v>103.8597186323054</v>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D78" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="79">
@@ -1745,10 +1725,8 @@
       <c r="C79" t="n">
         <v>103.849456501195</v>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D79" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="80">
@@ -1764,7 +1742,7 @@
         <v>103.838948514761</v>
       </c>
       <c r="D80" t="n">
-        <v>330</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81">
@@ -1780,7 +1758,7 @@
         <v>103.8512810718451</v>
       </c>
       <c r="D81" t="n">
-        <v>870</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="82">
@@ -1796,7 +1774,7 @@
         <v>103.8234022019441</v>
       </c>
       <c r="D82" t="n">
-        <v>5660</v>
+        <v>7720</v>
       </c>
     </row>
     <row r="83">
@@ -1811,10 +1789,8 @@
       <c r="C83" t="n">
         <v>103.8596907995843</v>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D83" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="84">
@@ -1830,7 +1806,7 @@
         <v>103.8496481250094</v>
       </c>
       <c r="D84" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85">
@@ -1846,7 +1822,7 @@
         <v>103.8475448562954</v>
       </c>
       <c r="D85" t="n">
-        <v>2440</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="86">
@@ -1880,7 +1856,7 @@
         <v>103.8081838596948</v>
       </c>
       <c r="D87" t="n">
-        <v>10560</v>
+        <v>24160</v>
       </c>
     </row>
     <row r="88">
@@ -1896,7 +1872,7 @@
         <v>103.8405375068011</v>
       </c>
       <c r="D88" t="n">
-        <v>1250</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="89">
@@ -1912,7 +1888,7 @@
         <v>103.8531680453032</v>
       </c>
       <c r="D89" t="n">
-        <v>510</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90">
@@ -1928,7 +1904,7 @@
         <v>103.8032270069761</v>
       </c>
       <c r="D90" t="n">
-        <v>8080</v>
+        <v>16480</v>
       </c>
     </row>
     <row r="91">
@@ -1944,7 +1920,7 @@
         <v>103.8340638293547</v>
       </c>
       <c r="D91" t="n">
-        <v>4050</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="92">
@@ -1959,10 +1935,8 @@
       <c r="C92" t="n">
         <v>103.7756118552405</v>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D92" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="93">
@@ -1978,7 +1952,7 @@
         <v>103.8451802703949</v>
       </c>
       <c r="D93" t="n">
-        <v>960</v>
+        <v>540</v>
       </c>
     </row>
     <row r="94">
@@ -1994,7 +1968,7 @@
         <v>103.8852042550787</v>
       </c>
       <c r="D94" t="n">
-        <v>12230</v>
+        <v>26850</v>
       </c>
     </row>
     <row r="95">
@@ -2010,7 +1984,7 @@
         <v>103.8586363593519</v>
       </c>
       <c r="D95" t="n">
-        <v>3400</v>
+        <v>8710</v>
       </c>
     </row>
     <row r="96">
@@ -2026,7 +2000,7 @@
         <v>103.9360163651932</v>
       </c>
       <c r="D96" t="n">
-        <v>32790</v>
+        <v>81550</v>
       </c>
     </row>
     <row r="97">
@@ -2042,7 +2016,7 @@
         <v>103.8459859257841</v>
       </c>
       <c r="D97" t="n">
-        <v>10770</v>
+        <v>27430</v>
       </c>
     </row>
     <row r="98">
@@ -2058,7 +2032,7 @@
         <v>103.7426809856293</v>
       </c>
       <c r="D98" t="n">
-        <v>770</v>
+        <v>580</v>
       </c>
     </row>
     <row r="99">
@@ -2074,7 +2048,7 @@
         <v>103.7837744520674</v>
       </c>
       <c r="D99" t="n">
-        <v>4870</v>
+        <v>11640</v>
       </c>
     </row>
     <row r="100">
@@ -2090,7 +2064,7 @@
         <v>103.8965728774673</v>
       </c>
       <c r="D100" t="n">
-        <v>4820</v>
+        <v>13690</v>
       </c>
     </row>
     <row r="101">
@@ -2106,7 +2080,7 @@
         <v>103.87362325664</v>
       </c>
       <c r="D101" t="n">
-        <v>6430</v>
+        <v>16580</v>
       </c>
     </row>
     <row r="102">
@@ -2122,7 +2096,7 @@
         <v>103.8656378602791</v>
       </c>
       <c r="D102" t="n">
-        <v>6000</v>
+        <v>12920</v>
       </c>
     </row>
     <row r="103">
@@ -2137,10 +2111,8 @@
       <c r="C103" t="n">
         <v>103.6512450611133</v>
       </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D103" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="104">
@@ -2156,7 +2128,7 @@
         <v>103.8586069551306</v>
       </c>
       <c r="D104" t="n">
-        <v>3990</v>
+        <v>9960</v>
       </c>
     </row>
     <row r="105">
@@ -2172,7 +2144,7 @@
         <v>103.8530251591554</v>
       </c>
       <c r="D105" t="n">
-        <v>6140</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="106">
@@ -2187,10 +2159,8 @@
       <c r="C106" t="n">
         <v>103.6979039975387</v>
       </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D106" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="107">
@@ -2224,7 +2194,7 @@
         <v>103.8521507588766</v>
       </c>
       <c r="D108" t="n">
-        <v>1250</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="109">
@@ -2240,7 +2210,7 @@
         <v>103.8385951940266</v>
       </c>
       <c r="D109" t="n">
-        <v>250</v>
+        <v>310</v>
       </c>
     </row>
     <row r="110">
@@ -2274,7 +2244,7 @@
         <v>103.8468130177092</v>
       </c>
       <c r="D111" t="n">
-        <v>2000</v>
+        <v>4850</v>
       </c>
     </row>
     <row r="112">
@@ -2290,7 +2260,7 @@
         <v>103.8396100841528</v>
       </c>
       <c r="D112" t="n">
-        <v>9030</v>
+        <v>21980</v>
       </c>
     </row>
     <row r="113">
@@ -2305,10 +2275,8 @@
       <c r="C113" t="n">
         <v>103.8647585285162</v>
       </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D113" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="114">
@@ -2378,7 +2346,7 @@
         <v>103.7874821188385</v>
       </c>
       <c r="D117" t="n">
-        <v>5500</v>
+        <v>13160</v>
       </c>
     </row>
     <row r="118">
@@ -2394,7 +2362,7 @@
         <v>103.8591397157486</v>
       </c>
       <c r="D118" t="n">
-        <v>6080</v>
+        <v>10190</v>
       </c>
     </row>
     <row r="119">
@@ -2410,7 +2378,7 @@
         <v>103.9204289719861</v>
       </c>
       <c r="D119" t="n">
-        <v>13890</v>
+        <v>35030</v>
       </c>
     </row>
     <row r="120">
@@ -2426,7 +2394,7 @@
         <v>103.7669448881544</v>
       </c>
       <c r="D120" t="n">
-        <v>12630</v>
+        <v>30800</v>
       </c>
     </row>
     <row r="121">
@@ -2442,7 +2410,7 @@
         <v>103.7969572361115</v>
       </c>
       <c r="D121" t="n">
-        <v>3820</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="122">
@@ -2458,7 +2426,7 @@
         <v>103.8983505669654</v>
       </c>
       <c r="D122" t="n">
-        <v>14840</v>
+        <v>32820</v>
       </c>
     </row>
     <row r="123">
@@ -2474,7 +2442,7 @@
         <v>103.7431555839674</v>
       </c>
       <c r="D123" t="n">
-        <v>6270</v>
+        <v>17480</v>
       </c>
     </row>
     <row r="124">
@@ -2508,7 +2476,7 @@
         <v>103.8702496554904</v>
       </c>
       <c r="D125" t="n">
-        <v>4430</v>
+        <v>10400</v>
       </c>
     </row>
     <row r="126">
@@ -2524,7 +2492,7 @@
         <v>103.8342972902919</v>
       </c>
       <c r="D126" t="n">
-        <v>930</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="127">
@@ -2539,10 +2507,8 @@
       <c r="C127" t="n">
         <v>103.7545033953382</v>
       </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D127" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="128">
@@ -2557,10 +2523,8 @@
       <c r="C128" t="n">
         <v>103.7771815246133</v>
       </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D128" t="n">
+        <v>160</v>
       </c>
     </row>
     <row r="129">
@@ -2576,7 +2540,7 @@
         <v>103.7630882474408</v>
       </c>
       <c r="D129" t="n">
-        <v>5900</v>
+        <v>14510</v>
       </c>
     </row>
     <row r="130">
@@ -2592,7 +2556,7 @@
         <v>103.8503615944201</v>
       </c>
       <c r="D130" t="n">
-        <v>5180</v>
+        <v>10390</v>
       </c>
     </row>
     <row r="131">
@@ -2608,7 +2572,7 @@
         <v>103.872300214973</v>
       </c>
       <c r="D131" t="n">
-        <v>4700</v>
+        <v>11980</v>
       </c>
     </row>
     <row r="132">
@@ -2623,10 +2587,8 @@
       <c r="C132" t="n">
         <v>103.8654799089959</v>
       </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D132" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="133">
@@ -2642,7 +2604,7 @@
         <v>103.7812925144643</v>
       </c>
       <c r="D133" t="n">
-        <v>4580</v>
+        <v>11290</v>
       </c>
     </row>
     <row r="134">
@@ -2658,7 +2620,7 @@
         <v>103.8051294388724</v>
       </c>
       <c r="D134" t="n">
-        <v>4020</v>
+        <v>7330</v>
       </c>
     </row>
     <row r="135">
@@ -2674,7 +2636,7 @@
         <v>103.8243572796261</v>
       </c>
       <c r="D135" t="n">
-        <v>5710</v>
+        <v>10580</v>
       </c>
     </row>
     <row r="136">
@@ -2690,7 +2652,7 @@
         <v>103.7550886341059</v>
       </c>
       <c r="D136" t="n">
-        <v>4480</v>
+        <v>10120</v>
       </c>
     </row>
     <row r="137">
@@ -2706,7 +2668,7 @@
         <v>103.9486507811498</v>
       </c>
       <c r="D137" t="n">
-        <v>4150</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="138">
@@ -2739,10 +2701,8 @@
       <c r="C139" t="n">
         <v>103.6688299024257</v>
       </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D139" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="140">
@@ -2758,7 +2718,7 @@
         <v>103.8129453381492</v>
       </c>
       <c r="D140" t="n">
-        <v>2330</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="141">
@@ -2774,7 +2734,7 @@
         <v>103.8428202353417</v>
       </c>
       <c r="D141" t="n">
-        <v>7320</v>
+        <v>11230</v>
       </c>
     </row>
     <row r="142">
@@ -2789,10 +2749,8 @@
       <c r="C142" t="n">
         <v>103.7082322313242</v>
       </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D142" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="143">
@@ -2808,7 +2766,7 @@
         <v>103.8257966275489</v>
       </c>
       <c r="D143" t="n">
-        <v>800</v>
+        <v>580</v>
       </c>
     </row>
     <row r="144">
@@ -2824,7 +2782,7 @@
         <v>103.9075742506078</v>
       </c>
       <c r="D144" t="n">
-        <v>13410</v>
+        <v>27140</v>
       </c>
     </row>
     <row r="145">
@@ -2839,10 +2797,8 @@
       <c r="C145" t="n">
         <v>103.6795217712566</v>
       </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D145" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="146">
@@ -2857,10 +2813,8 @@
       <c r="C146" t="n">
         <v>103.8761038318087</v>
       </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D146" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="147">
@@ -2875,10 +2829,8 @@
       <c r="C147" t="n">
         <v>103.7480871239683</v>
       </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D147" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="148">
@@ -2893,10 +2845,8 @@
       <c r="C148" t="n">
         <v>103.7092505073348</v>
       </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D148" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="149">
@@ -2912,7 +2862,7 @@
         <v>103.8015380549468</v>
       </c>
       <c r="D149" t="n">
-        <v>2810</v>
+        <v>7480</v>
       </c>
     </row>
     <row r="150">
@@ -2928,7 +2878,7 @@
         <v>103.9156144222308</v>
       </c>
       <c r="D150" t="n">
-        <v>13850</v>
+        <v>35890</v>
       </c>
     </row>
     <row r="151">
@@ -2944,7 +2894,7 @@
         <v>103.8200696432102</v>
       </c>
       <c r="D151" t="n">
-        <v>1480</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="152">
@@ -2960,7 +2910,7 @@
         <v>103.7686678697861</v>
       </c>
       <c r="D152" t="n">
-        <v>2060</v>
+        <v>5470</v>
       </c>
     </row>
     <row r="153">
@@ -2976,7 +2926,7 @@
         <v>103.7715703486618</v>
       </c>
       <c r="D153" t="n">
-        <v>8370</v>
+        <v>22960</v>
       </c>
     </row>
     <row r="154">
@@ -2992,7 +2942,7 @@
         <v>103.792304821283</v>
       </c>
       <c r="D154" t="n">
-        <v>2420</v>
+        <v>6110</v>
       </c>
     </row>
     <row r="155">
@@ -3008,7 +2958,7 @@
         <v>103.9688107674251</v>
       </c>
       <c r="D155" t="n">
-        <v>810</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="156">
@@ -3024,7 +2974,7 @@
         <v>103.7568486581327</v>
       </c>
       <c r="D156" t="n">
-        <v>3520</v>
+        <v>8060</v>
       </c>
     </row>
     <row r="157">
@@ -3040,7 +2990,7 @@
         <v>103.8339408435598</v>
       </c>
       <c r="D157" t="n">
-        <v>1190</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="158">
@@ -3056,7 +3006,7 @@
         <v>103.9445541269731</v>
       </c>
       <c r="D158" t="n">
-        <v>18830</v>
+        <v>48360</v>
       </c>
     </row>
     <row r="159">
@@ -3071,10 +3021,8 @@
       <c r="C159" t="n">
         <v>103.8957813832331</v>
       </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D159" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="160">
@@ -3126,7 +3074,7 @@
         <v>103.7480037864719</v>
       </c>
       <c r="D162" t="n">
-        <v>8820</v>
+        <v>25140</v>
       </c>
     </row>
     <row r="163">
@@ -3142,7 +3090,7 @@
         <v>103.880680210422</v>
       </c>
       <c r="D163" t="n">
-        <v>10190</v>
+        <v>27280</v>
       </c>
     </row>
     <row r="164">
@@ -3158,7 +3106,7 @@
         <v>103.8556525913375</v>
       </c>
       <c r="D164" t="n">
-        <v>10110</v>
+        <v>25190</v>
       </c>
     </row>
     <row r="165">
@@ -3174,7 +3122,7 @@
         <v>103.8666628375142</v>
       </c>
       <c r="D165" t="n">
-        <v>13920</v>
+        <v>37450</v>
       </c>
     </row>
     <row r="166">
@@ -3190,7 +3138,7 @@
         <v>103.8914623634855</v>
       </c>
       <c r="D166" t="n">
-        <v>1630</v>
+        <v>4720</v>
       </c>
     </row>
     <row r="167">
@@ -3206,7 +3154,7 @@
         <v>103.973426810157</v>
       </c>
       <c r="D167" t="n">
-        <v>720</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="168">
@@ -3222,7 +3170,7 @@
         <v>103.7720461919587</v>
       </c>
       <c r="D168" t="n">
-        <v>3160</v>
+        <v>7860</v>
       </c>
     </row>
     <row r="169">
@@ -3238,7 +3186,7 @@
         <v>103.9594106485448</v>
       </c>
       <c r="D169" t="n">
-        <v>15570</v>
+        <v>51680</v>
       </c>
     </row>
     <row r="170">
@@ -3254,7 +3202,7 @@
         <v>103.9390256518351</v>
       </c>
       <c r="D170" t="n">
-        <v>11390</v>
+        <v>32830</v>
       </c>
     </row>
     <row r="171">
@@ -3270,7 +3218,7 @@
         <v>103.8540952773522</v>
       </c>
       <c r="D171" t="n">
-        <v>10990</v>
+        <v>26970</v>
       </c>
     </row>
     <row r="172">
@@ -3286,7 +3234,7 @@
         <v>103.8307659503001</v>
       </c>
       <c r="D172" t="n">
-        <v>2080</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="173">
@@ -3302,7 +3250,7 @@
         <v>103.7662436525526</v>
       </c>
       <c r="D173" t="n">
-        <v>10430</v>
+        <v>29960</v>
       </c>
     </row>
     <row r="174">
@@ -3318,7 +3266,7 @@
         <v>103.7464596658592</v>
       </c>
       <c r="D174" t="n">
-        <v>12190</v>
+        <v>39370</v>
       </c>
     </row>
     <row r="175">
@@ -3334,7 +3282,7 @@
         <v>103.8618562383587</v>
       </c>
       <c r="D175" t="n">
-        <v>16030</v>
+        <v>36790</v>
       </c>
     </row>
     <row r="176">
@@ -3350,7 +3298,7 @@
         <v>103.8510673949843</v>
       </c>
       <c r="D176" t="n">
-        <v>15970</v>
+        <v>32690</v>
       </c>
     </row>
     <row r="177">
@@ -3365,10 +3313,8 @@
       <c r="C177" t="n">
         <v>103.6330033731129</v>
       </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D177" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="178">
@@ -3384,7 +3330,7 @@
         <v>103.870675243507</v>
       </c>
       <c r="D178" t="n">
-        <v>9460</v>
+        <v>22590</v>
       </c>
     </row>
     <row r="179">
@@ -3400,7 +3346,7 @@
         <v>103.8530142619292</v>
       </c>
       <c r="D179" t="n">
-        <v>9930</v>
+        <v>27460</v>
       </c>
     </row>
     <row r="180">
@@ -3416,7 +3362,7 @@
         <v>103.9359493740577</v>
       </c>
       <c r="D180" t="n">
-        <v>29070</v>
+        <v>83260</v>
       </c>
     </row>
     <row r="181">
@@ -3432,7 +3378,7 @@
         <v>103.7421947724281</v>
       </c>
       <c r="D181" t="n">
-        <v>11800</v>
+        <v>31090</v>
       </c>
     </row>
     <row r="182">
@@ -3448,7 +3394,7 @@
         <v>103.8733841355309</v>
       </c>
       <c r="D182" t="n">
-        <v>4650</v>
+        <v>15200</v>
       </c>
     </row>
     <row r="183">
@@ -3464,7 +3410,7 @@
         <v>103.7538120225021</v>
       </c>
       <c r="D183" t="n">
-        <v>4900</v>
+        <v>12830</v>
       </c>
     </row>
     <row r="184">
@@ -3480,7 +3426,7 @@
         <v>103.7071019757341</v>
       </c>
       <c r="D184" t="n">
-        <v>2370</v>
+        <v>8180</v>
       </c>
     </row>
     <row r="185">
@@ -3496,7 +3442,7 @@
         <v>103.7778109120893</v>
       </c>
       <c r="D185" t="n">
-        <v>1550</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="186">
@@ -3512,7 +3458,7 @@
         <v>103.9512415711453</v>
       </c>
       <c r="D186" t="n">
-        <v>43870</v>
+        <v>128250</v>
       </c>
     </row>
     <row r="187">
@@ -3528,7 +3474,7 @@
         <v>103.8866063626297</v>
       </c>
       <c r="D187" t="n">
-        <v>12360</v>
+        <v>31590</v>
       </c>
     </row>
     <row r="188">
@@ -3544,7 +3490,7 @@
         <v>103.9663218852747</v>
       </c>
       <c r="D188" t="n">
-        <v>6860</v>
+        <v>16290</v>
       </c>
     </row>
     <row r="189">
@@ -3560,7 +3506,7 @@
         <v>103.7639224210027</v>
       </c>
       <c r="D189" t="n">
-        <v>8680</v>
+        <v>20660</v>
       </c>
     </row>
     <row r="190">
@@ -3575,10 +3521,8 @@
       <c r="C190" t="n">
         <v>103.756340422445</v>
       </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D190" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="191">
@@ -3594,7 +3538,7 @@
         <v>103.8289703131776</v>
       </c>
       <c r="D191" t="n">
-        <v>240</v>
+        <v>700</v>
       </c>
     </row>
     <row r="192">
@@ -3610,7 +3554,7 @@
         <v>103.8082294562253</v>
       </c>
       <c r="D192" t="n">
-        <v>3640</v>
+        <v>9870</v>
       </c>
     </row>
     <row r="193">
@@ -3626,7 +3570,7 @@
         <v>103.8823265529691</v>
       </c>
       <c r="D193" t="n">
-        <v>3320</v>
+        <v>7920</v>
       </c>
     </row>
     <row r="194">
@@ -3660,7 +3604,7 @@
         <v>103.857102042756</v>
       </c>
       <c r="D195" t="n">
-        <v>2690</v>
+        <v>6720</v>
       </c>
     </row>
     <row r="196">
@@ -3676,7 +3620,7 @@
         <v>103.7461061215432</v>
       </c>
       <c r="D196" t="n">
-        <v>4610</v>
+        <v>13830</v>
       </c>
     </row>
     <row r="197">
@@ -3692,7 +3636,7 @@
         <v>103.9540028421885</v>
       </c>
       <c r="D197" t="n">
-        <v>13970</v>
+        <v>38470</v>
       </c>
     </row>
     <row r="198">
@@ -3708,7 +3652,7 @@
         <v>103.7111482623445</v>
       </c>
       <c r="D198" t="n">
-        <v>10860</v>
+        <v>29510</v>
       </c>
     </row>
     <row r="199">
@@ -3724,7 +3668,7 @@
         <v>103.7575370687177</v>
       </c>
       <c r="D199" t="n">
-        <v>4570</v>
+        <v>12070</v>
       </c>
     </row>
     <row r="200">
@@ -3740,7 +3684,7 @@
         <v>103.7422490270435</v>
       </c>
       <c r="D200" t="n">
-        <v>5060</v>
+        <v>14350</v>
       </c>
     </row>
     <row r="201">
@@ -3756,7 +3700,7 @@
         <v>103.7504132760217</v>
       </c>
       <c r="D201" t="n">
-        <v>9770</v>
+        <v>27320</v>
       </c>
     </row>
     <row r="202">
@@ -3772,7 +3716,7 @@
         <v>103.8770472624619</v>
       </c>
       <c r="D202" t="n">
-        <v>7670</v>
+        <v>18430</v>
       </c>
     </row>
     <row r="203">
@@ -3788,7 +3732,7 @@
         <v>103.8876193790896</v>
       </c>
       <c r="D203" t="n">
-        <v>4370</v>
+        <v>12950</v>
       </c>
     </row>
     <row r="204">
@@ -3822,7 +3766,7 @@
         <v>103.7319720986947</v>
       </c>
       <c r="D205" t="n">
-        <v>6980</v>
+        <v>18550</v>
       </c>
     </row>
     <row r="206">
@@ -3838,7 +3782,7 @@
         <v>103.8495968905182</v>
       </c>
       <c r="D206" t="n">
-        <v>3850</v>
+        <v>9530</v>
       </c>
     </row>
     <row r="207">
@@ -3854,7 +3798,7 @@
         <v>103.874944712625</v>
       </c>
       <c r="D207" t="n">
-        <v>3350</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="208">
@@ -3870,7 +3814,7 @@
         <v>103.8663000048399</v>
       </c>
       <c r="D208" t="n">
-        <v>1900</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="209">
@@ -3886,7 +3830,7 @@
         <v>103.721196983089</v>
       </c>
       <c r="D209" t="n">
-        <v>13900</v>
+        <v>39010</v>
       </c>
     </row>
     <row r="210">
@@ -3902,7 +3846,7 @@
         <v>103.7284787600249</v>
       </c>
       <c r="D210" t="n">
-        <v>140</v>
+        <v>550</v>
       </c>
     </row>
     <row r="211">
@@ -3918,7 +3862,7 @@
         <v>103.8417937230166</v>
       </c>
       <c r="D211" t="n">
-        <v>6130</v>
+        <v>13960</v>
       </c>
     </row>
     <row r="212">
@@ -3934,7 +3878,7 @@
         <v>103.9095646429237</v>
       </c>
       <c r="D212" t="n">
-        <v>12550</v>
+        <v>35440</v>
       </c>
     </row>
     <row r="213">
@@ -3950,7 +3894,7 @@
         <v>103.7388366679664</v>
       </c>
       <c r="D213" t="n">
-        <v>8840</v>
+        <v>23530</v>
       </c>
     </row>
     <row r="214">
@@ -3966,7 +3910,7 @@
         <v>103.7581260664141</v>
       </c>
       <c r="D214" t="n">
-        <v>4630</v>
+        <v>14520</v>
       </c>
     </row>
     <row r="215">
@@ -3982,7 +3926,7 @@
         <v>103.7020987055076</v>
       </c>
       <c r="D215" t="n">
-        <v>19660</v>
+        <v>61900</v>
       </c>
     </row>
     <row r="216">
@@ -3998,7 +3942,7 @@
         <v>103.9263294641104</v>
       </c>
       <c r="D216" t="n">
-        <v>9470</v>
+        <v>25190</v>
       </c>
     </row>
     <row r="217">
@@ -4014,7 +3958,7 @@
         <v>103.8462370960546</v>
       </c>
       <c r="D217" t="n">
-        <v>6150</v>
+        <v>19150</v>
       </c>
     </row>
     <row r="218">
@@ -4030,7 +3974,7 @@
         <v>103.9067737092831</v>
       </c>
       <c r="D218" t="n">
-        <v>9500</v>
+        <v>18420</v>
       </c>
     </row>
     <row r="219">
@@ -4046,7 +3990,7 @@
         <v>103.8250757777259</v>
       </c>
       <c r="D219" t="n">
-        <v>690</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="220">
@@ -4062,7 +4006,7 @@
         <v>103.837659411632</v>
       </c>
       <c r="D220" t="n">
-        <v>1310</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="221">
@@ -4078,7 +4022,7 @@
         <v>103.9479393583852</v>
       </c>
       <c r="D221" t="n">
-        <v>11260</v>
+        <v>31730</v>
       </c>
     </row>
     <row r="222">
@@ -4094,7 +4038,7 @@
         <v>103.7574756054059</v>
       </c>
       <c r="D222" t="n">
-        <v>3310</v>
+        <v>9770</v>
       </c>
     </row>
     <row r="223">
@@ -4109,10 +4053,8 @@
       <c r="C223" t="n">
         <v>103.9258001901725</v>
       </c>
-      <c r="D223" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D223" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="224">
@@ -4128,7 +4070,7 @@
         <v>103.8973688434884</v>
       </c>
       <c r="D224" t="n">
-        <v>8000</v>
+        <v>23800</v>
       </c>
     </row>
     <row r="225">
@@ -4162,7 +4104,7 @@
         <v>103.8982172846148</v>
       </c>
       <c r="D226" t="n">
-        <v>13710</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="227">
@@ -4178,7 +4120,7 @@
         <v>103.9778348289413</v>
       </c>
       <c r="D227" t="n">
-        <v>110</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="228">
@@ -4194,7 +4136,7 @@
         <v>103.7946159472667</v>
       </c>
       <c r="D228" t="n">
-        <v>5570</v>
+        <v>12010</v>
       </c>
     </row>
     <row r="229">
@@ -4210,7 +4152,7 @@
         <v>103.8858780214234</v>
       </c>
       <c r="D229" t="n">
-        <v>14920</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="230">
@@ -4244,7 +4186,7 @@
         <v>103.7742933758073</v>
       </c>
       <c r="D231" t="n">
-        <v>7070</v>
+        <v>21010</v>
       </c>
     </row>
     <row r="232">
@@ -4278,7 +4220,7 @@
         <v>103.7386295287879</v>
       </c>
       <c r="D233" t="n">
-        <v>10150</v>
+        <v>33860</v>
       </c>
     </row>
     <row r="234">
@@ -4294,7 +4236,7 @@
         <v>103.9398121881611</v>
       </c>
       <c r="D234" t="n">
-        <v>10810</v>
+        <v>34970</v>
       </c>
     </row>
     <row r="235">
@@ -4310,7 +4252,7 @@
         <v>103.8400623624617</v>
       </c>
       <c r="D235" t="n">
-        <v>9610</v>
+        <v>23570</v>
       </c>
     </row>
     <row r="236">
@@ -4326,7 +4268,7 @@
         <v>103.9825240414284</v>
       </c>
       <c r="D236" t="n">
-        <v>340</v>
+        <v>560</v>
       </c>
     </row>
     <row r="237">
@@ -4342,7 +4284,7 @@
         <v>103.8976845596669</v>
       </c>
       <c r="D237" t="n">
-        <v>19780</v>
+        <v>60500</v>
       </c>
     </row>
     <row r="238">
@@ -4358,7 +4300,7 @@
         <v>103.8891893554625</v>
       </c>
       <c r="D238" t="n">
-        <v>17170</v>
+        <v>51310</v>
       </c>
     </row>
     <row r="239">
@@ -4392,7 +4334,7 @@
         <v>103.8765052469368</v>
       </c>
       <c r="D240" t="n">
-        <v>26020</v>
+        <v>69010</v>
       </c>
     </row>
     <row r="241">
@@ -4408,7 +4350,7 @@
         <v>103.9112604488021</v>
       </c>
       <c r="D241" t="n">
-        <v>15720</v>
+        <v>48540</v>
       </c>
     </row>
     <row r="242">
@@ -4424,7 +4366,7 @@
         <v>103.7479363747593</v>
       </c>
       <c r="D242" t="n">
-        <v>12070</v>
+        <v>39620</v>
       </c>
     </row>
     <row r="243">
@@ -4439,10 +4381,8 @@
       <c r="C243" t="n">
         <v>103.9286800442584</v>
       </c>
-      <c r="D243" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D243" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="244">
@@ -4458,7 +4398,7 @@
         <v>103.8814059848753</v>
       </c>
       <c r="D244" t="n">
-        <v>15910</v>
+        <v>49090</v>
       </c>
     </row>
     <row r="245">
@@ -4474,7 +4414,7 @@
         <v>103.7548706384115</v>
       </c>
       <c r="D245" t="n">
-        <v>8530</v>
+        <v>24560</v>
       </c>
     </row>
     <row r="246">
@@ -4490,7 +4430,7 @@
         <v>103.7476369390366</v>
       </c>
       <c r="D246" t="n">
-        <v>6880</v>
+        <v>21980</v>
       </c>
     </row>
     <row r="247">
@@ -4506,7 +4446,7 @@
         <v>103.7711457395419</v>
       </c>
       <c r="D247" t="n">
-        <v>8250</v>
+        <v>26420</v>
       </c>
     </row>
     <row r="248">
@@ -4522,7 +4462,7 @@
         <v>103.7605154537585</v>
       </c>
       <c r="D248" t="n">
-        <v>8210</v>
+        <v>23830</v>
       </c>
     </row>
     <row r="249">
@@ -4538,7 +4478,7 @@
         <v>103.7662552671834</v>
       </c>
       <c r="D249" t="n">
-        <v>7540</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="250">
@@ -4554,7 +4494,7 @@
         <v>103.8663588591855</v>
       </c>
       <c r="D250" t="n">
-        <v>4830</v>
+        <v>15390</v>
       </c>
     </row>
     <row r="251">
@@ -4570,7 +4510,7 @@
         <v>103.8899670442132</v>
       </c>
       <c r="D251" t="n">
-        <v>7970</v>
+        <v>21580</v>
       </c>
     </row>
     <row r="252">
@@ -4586,7 +4526,7 @@
         <v>103.8533960645811</v>
       </c>
       <c r="D252" t="n">
-        <v>1430</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="253">
@@ -4601,10 +4541,8 @@
       <c r="C253" t="n">
         <v>103.8462917270462</v>
       </c>
-      <c r="D253" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D253" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="254">
@@ -4619,10 +4557,8 @@
       <c r="C254" t="n">
         <v>103.9707356852154</v>
       </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D254" t="n">
+        <v>540</v>
       </c>
     </row>
     <row r="255">
@@ -4638,7 +4574,7 @@
         <v>103.8283384102957</v>
       </c>
       <c r="D255" t="n">
-        <v>2530</v>
+        <v>7980</v>
       </c>
     </row>
     <row r="256">
@@ -4654,7 +4590,7 @@
         <v>103.9548937377897</v>
       </c>
       <c r="D256" t="n">
-        <v>3280</v>
+        <v>7890</v>
       </c>
     </row>
     <row r="257">
@@ -4670,7 +4606,7 @@
         <v>103.7465839041033</v>
       </c>
       <c r="D257" t="n">
-        <v>9020</v>
+        <v>30790</v>
       </c>
     </row>
     <row r="258">
@@ -4686,7 +4622,7 @@
         <v>103.9050035466765</v>
       </c>
       <c r="D258" t="n">
-        <v>21080</v>
+        <v>62660</v>
       </c>
     </row>
     <row r="259">
@@ -4720,7 +4656,7 @@
         <v>103.6948786977978</v>
       </c>
       <c r="D260" t="n">
-        <v>19990</v>
+        <v>66560</v>
       </c>
     </row>
     <row r="261">
@@ -4736,7 +4672,7 @@
         <v>103.8632205994803</v>
       </c>
       <c r="D261" t="n">
-        <v>3110</v>
+        <v>8550</v>
       </c>
     </row>
     <row r="262">
@@ -4752,7 +4688,7 @@
         <v>103.721069575677</v>
       </c>
       <c r="D262" t="n">
-        <v>18860</v>
+        <v>52260</v>
       </c>
     </row>
     <row r="263">
@@ -4768,7 +4704,7 @@
         <v>103.8815865289379</v>
       </c>
       <c r="D263" t="n">
-        <v>130</v>
+        <v>290</v>
       </c>
     </row>
     <row r="264">
@@ -4783,10 +4719,8 @@
       <c r="C264" t="n">
         <v>103.7482724939851</v>
       </c>
-      <c r="D264" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D264" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="265">
@@ -4801,10 +4735,8 @@
       <c r="C265" t="n">
         <v>103.8664803731979</v>
       </c>
-      <c r="D265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D265" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="266">
@@ -4820,7 +4752,7 @@
         <v>103.8286516323082</v>
       </c>
       <c r="D266" t="n">
-        <v>3490</v>
+        <v>9810</v>
       </c>
     </row>
     <row r="267">
@@ -4872,7 +4804,7 @@
         <v>103.8378164444206</v>
       </c>
       <c r="D269" t="n">
-        <v>14200</v>
+        <v>41490</v>
       </c>
     </row>
     <row r="270">
@@ -4887,10 +4819,8 @@
       <c r="C270" t="n">
         <v>103.7467585938742</v>
       </c>
-      <c r="D270" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D270" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="271">
@@ -4906,7 +4836,7 @@
         <v>103.8019273073558</v>
       </c>
       <c r="D271" t="n">
-        <v>29940</v>
+        <v>99870</v>
       </c>
     </row>
     <row r="272">
@@ -4922,7 +4852,7 @@
         <v>103.8177676394977</v>
       </c>
       <c r="D272" t="n">
-        <v>11230</v>
+        <v>35400</v>
       </c>
     </row>
     <row r="273">
@@ -4937,10 +4867,8 @@
       <c r="C273" t="n">
         <v>103.7848695707179</v>
       </c>
-      <c r="D273" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D273" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="274">
@@ -4956,7 +4884,7 @@
         <v>103.8314219948951</v>
       </c>
       <c r="D274" t="n">
-        <v>8770</v>
+        <v>23480</v>
       </c>
     </row>
     <row r="275">
@@ -4971,10 +4899,8 @@
       <c r="C275" t="n">
         <v>103.7966695788419</v>
       </c>
-      <c r="D275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D275" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="276">
@@ -4990,7 +4916,7 @@
         <v>103.8970208924133</v>
       </c>
       <c r="D276" t="n">
-        <v>18330</v>
+        <v>52960</v>
       </c>
     </row>
     <row r="277">
@@ -5006,7 +4932,7 @@
         <v>103.9147590578205</v>
       </c>
       <c r="D277" t="n">
-        <v>18490</v>
+        <v>54260</v>
       </c>
     </row>
     <row r="278">
@@ -5021,10 +4947,8 @@
       <c r="C278" t="n">
         <v>103.7629153382516</v>
       </c>
-      <c r="D278" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D278" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="279">
@@ -5040,7 +4964,7 @@
         <v>103.8629399211811</v>
       </c>
       <c r="D279" t="n">
-        <v>4660</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="280">
@@ -5055,10 +4979,8 @@
       <c r="C280" t="n">
         <v>103.6431996182845</v>
       </c>
-      <c r="D280" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D280" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="281">
@@ -5073,10 +4995,8 @@
       <c r="C281" t="n">
         <v>103.6313817890389</v>
       </c>
-      <c r="D281" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D281" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="282">
@@ -5200,7 +5120,7 @@
         <v>103.7342360740744</v>
       </c>
       <c r="D288" t="n">
-        <v>5060</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="289">
@@ -5216,7 +5136,7 @@
         <v>103.7284216150547</v>
       </c>
       <c r="D289" t="n">
-        <v>960</v>
+        <v>280</v>
       </c>
     </row>
     <row r="290">
@@ -5250,7 +5170,7 @@
         <v>103.7807246067226</v>
       </c>
       <c r="D291" t="n">
-        <v>3900</v>
+        <v>11430</v>
       </c>
     </row>
     <row r="292">
@@ -5266,7 +5186,7 @@
         <v>103.8240606933011</v>
       </c>
       <c r="D292" t="n">
-        <v>1300</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="293">
@@ -5282,7 +5202,7 @@
         <v>103.9016478351457</v>
       </c>
       <c r="D293" t="n">
-        <v>8920</v>
+        <v>25220</v>
       </c>
     </row>
     <row r="294">
@@ -5334,7 +5254,7 @@
         <v>103.8364859598911</v>
       </c>
       <c r="D296" t="n">
-        <v>740</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="297">
@@ -5367,10 +5287,8 @@
       <c r="C298" t="n">
         <v>103.8033579090288</v>
       </c>
-      <c r="D298" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D298" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="299">
@@ -5404,7 +5322,7 @@
         <v>103.8408050542332</v>
       </c>
       <c r="D300" t="n">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="301">
@@ -5420,7 +5338,7 @@
         <v>103.8912776678921</v>
       </c>
       <c r="D301" t="n">
-        <v>4430</v>
+        <v>10100</v>
       </c>
     </row>
     <row r="302">
@@ -5436,7 +5354,7 @@
         <v>103.8835734427831</v>
       </c>
       <c r="D302" t="n">
-        <v>22830</v>
+        <v>43210</v>
       </c>
     </row>
     <row r="303">
@@ -5470,7 +5388,7 @@
         <v>103.7635395814467</v>
       </c>
       <c r="D304" t="n">
-        <v>220</v>
+        <v>680</v>
       </c>
     </row>
     <row r="305">
@@ -5486,7 +5404,7 @@
         <v>103.7938665101297</v>
       </c>
       <c r="D305" t="n">
-        <v>12330</v>
+        <v>40150</v>
       </c>
     </row>
     <row r="306">
@@ -5502,7 +5420,7 @@
         <v>103.7785498460008</v>
       </c>
       <c r="D306" t="n">
-        <v>10330</v>
+        <v>32670</v>
       </c>
     </row>
     <row r="307">
@@ -5518,7 +5436,7 @@
         <v>103.8465855719554</v>
       </c>
       <c r="D307" t="n">
-        <v>24890</v>
+        <v>71930</v>
       </c>
     </row>
     <row r="308">
@@ -5533,10 +5451,8 @@
       <c r="C308" t="n">
         <v>103.6896286985971</v>
       </c>
-      <c r="D308" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D308" t="n">
+        <v>600</v>
       </c>
     </row>
     <row r="309">
@@ -5588,7 +5504,7 @@
         <v>103.8251527593361</v>
       </c>
       <c r="D311" t="n">
-        <v>4670</v>
+        <v>13530</v>
       </c>
     </row>
     <row r="312">
@@ -5603,10 +5519,8 @@
       <c r="C312" t="n">
         <v>103.7192852380507</v>
       </c>
-      <c r="D312" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D312" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="313">
@@ -5639,10 +5553,8 @@
       <c r="C314" t="n">
         <v>103.8075381353528</v>
       </c>
-      <c r="D314" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D314" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="315">
@@ -5658,7 +5570,7 @@
         <v>103.8156962040599</v>
       </c>
       <c r="D315" t="n">
-        <v>8010</v>
+        <v>25730</v>
       </c>
     </row>
     <row r="316">
@@ -5692,7 +5604,7 @@
         <v>103.8310115889117</v>
       </c>
       <c r="D317" t="n">
-        <v>18870</v>
+        <v>51760</v>
       </c>
     </row>
     <row r="318">
@@ -5725,10 +5637,8 @@
       <c r="C319" t="n">
         <v>104.0348229111765</v>
       </c>
-      <c r="D319" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D319" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="320">
@@ -5762,7 +5672,7 @@
         <v>103.8379965032943</v>
       </c>
       <c r="D321" t="n">
-        <v>9310</v>
+        <v>27080</v>
       </c>
     </row>
     <row r="322">
@@ -5778,7 +5688,7 @@
         <v>103.7915316582188</v>
       </c>
       <c r="D322" t="n">
-        <v>9670</v>
+        <v>34380</v>
       </c>
     </row>
     <row r="323">
@@ -5794,7 +5704,7 @@
         <v>103.775651993175</v>
       </c>
       <c r="D323" t="n">
-        <v>12940</v>
+        <v>36550</v>
       </c>
     </row>
     <row r="324">
@@ -5810,7 +5720,7 @@
         <v>103.8250228336302</v>
       </c>
       <c r="D324" t="n">
-        <v>3140</v>
+        <v>9540</v>
       </c>
     </row>
     <row r="325">
@@ -5880,7 +5790,7 @@
         <v>103.814643374198</v>
       </c>
       <c r="D328" t="n">
-        <v>420</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="329">
@@ -5896,7 +5806,7 @@
         <v>103.832301064889</v>
       </c>
       <c r="D329" t="n">
-        <v>11980</v>
+        <v>31670</v>
       </c>
     </row>
     <row r="330">
@@ -5912,7 +5822,7 @@
         <v>103.8383928790692</v>
       </c>
       <c r="D330" t="n">
-        <v>6940</v>
+        <v>17460</v>
       </c>
     </row>
     <row r="331">
@@ -5928,7 +5838,7 @@
         <v>103.8484725568306</v>
       </c>
       <c r="D331" t="n">
-        <v>8030</v>
+        <v>20010</v>
       </c>
     </row>
     <row r="332">
@@ -5944,7 +5854,7 @@
         <v>103.844888415435</v>
       </c>
       <c r="D332" t="n">
-        <v>9310</v>
+        <v>28800</v>
       </c>
     </row>
     <row r="333">
@@ -5959,10 +5869,8 @@
       <c r="C333" t="n">
         <v>103.6276062586927</v>
       </c>
-      <c r="D333" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D333" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>